<commit_message>
updates to use_cases.xlsx and table_column_names.xlsx
</commit_message>
<xml_diff>
--- a/Load CSV files/table_column_names.xlsx
+++ b/Load CSV files/table_column_names.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,20 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bill\Desktop\Syracuse_MIS\IST 659\sql_project\Load CSV files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{698D1503-DCA9-4D09-B6BF-BE551B3C4711}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9EC1FBC-7A40-4D85-998D-F646EA6904E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="1"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="players" sheetId="2" r:id="rId1"/>
     <sheet name="cards" sheetId="4" r:id="rId2"/>
+    <sheet name="bills_cards" sheetId="5" r:id="rId3"/>
+    <sheet name="teams" sheetId="6" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="64">
   <si>
     <t>player_name</t>
   </si>
@@ -162,12 +177,63 @@
   </si>
   <si>
     <t>FK</t>
+  </si>
+  <si>
+    <t>bills_card_cert</t>
+  </si>
+  <si>
+    <t>bills_card_spec</t>
+  </si>
+  <si>
+    <t>bills_card_num</t>
+  </si>
+  <si>
+    <t>bills_card_year</t>
+  </si>
+  <si>
+    <t>bills_card_psa_desc</t>
+  </si>
+  <si>
+    <t>bills_card_grade</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>bills_card_pop</t>
+  </si>
+  <si>
+    <t>bills_card_pop_higher</t>
+  </si>
+  <si>
+    <t>bills_card_stat_year</t>
+  </si>
+  <si>
+    <t>bills_card_player_id</t>
+  </si>
+  <si>
+    <t>bills_card_id</t>
+  </si>
+  <si>
+    <t>team_code</t>
+  </si>
+  <si>
+    <t>char</t>
+  </si>
+  <si>
+    <t>team_city</t>
+  </si>
+  <si>
+    <t>team_name</t>
+  </si>
+  <si>
+    <t>team_league</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -666,11 +732,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1025,7 +1092,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1376,11 +1443,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1497,4 +1564,259 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DE29E5D-DC79-4677-AA27-B2D1DD13DCE9}">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="4.7890625" customWidth="1"/>
+    <col min="2" max="2" width="18.9453125" customWidth="1"/>
+    <col min="3" max="3" width="7" customWidth="1"/>
+    <col min="4" max="4" width="10.20703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="3"/>
+      <c r="B4" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="3"/>
+      <c r="B5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="3"/>
+      <c r="B6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="3"/>
+      <c r="B7" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="3"/>
+      <c r="B8" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="3"/>
+      <c r="B9" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="3"/>
+      <c r="B10" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="3"/>
+      <c r="B11" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{830D24AB-91DD-4132-98BB-C490735FD941}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="4.05078125" customWidth="1"/>
+    <col min="2" max="2" width="14.1015625" customWidth="1"/>
+    <col min="3" max="3" width="6.83984375" customWidth="1"/>
+    <col min="4" max="4" width="10.20703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="4"/>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>